<commit_message>
Pre-simplifying of dropPiece function => either incorrect index on turn (feature) or shapes wont drop (bug)
</commit_message>
<xml_diff>
--- a/tetrisShapeRotations.xlsx
+++ b/tetrisShapeRotations.xlsx
@@ -375,7 +375,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -474,6 +474,9 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -913,8 +916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="G2:AL35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="W29" sqref="W29"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.83203125" defaultRowHeight="35" customHeight="1" x14ac:dyDescent="0"/>
@@ -1556,7 +1559,7 @@
       <c r="N27" s="21"/>
       <c r="O27" s="21"/>
       <c r="P27" s="22"/>
-      <c r="R27" s="20"/>
+      <c r="R27" s="34"/>
       <c r="S27" s="5"/>
       <c r="T27" s="5"/>
       <c r="U27" s="22"/>

</xml_diff>

<commit_message>
Updated link to game, footer font, removed set height width from gameboard
</commit_message>
<xml_diff>
--- a/tetrisShapeRotations.xlsx
+++ b/tetrisShapeRotations.xlsx
@@ -19,19 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="32">
-  <si>
-    <t>index</t>
-  </si>
-  <si>
-    <t>index+1</t>
-  </si>
-  <si>
-    <t>index+2</t>
-  </si>
-  <si>
-    <t>index+3</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="27">
   <si>
     <t>I: [index, index+width, index+(2*width), index+(3*width)],</t>
   </si>
@@ -112,9 +100,6 @@
   </si>
   <si>
     <t>i3w+2</t>
-  </si>
-  <si>
-    <t>i2w+2</t>
   </si>
 </sst>
 </file>
@@ -268,8 +253,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="105">
+  <cellStyleXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -480,7 +467,7 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="105">
+  <cellStyles count="107">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -533,6 +520,7 @@
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -585,6 +573,7 @@
     <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -916,8 +905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="G2:AL35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="R27" sqref="R27"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.83203125" defaultRowHeight="35" customHeight="1" x14ac:dyDescent="0"/>
@@ -932,19 +921,19 @@
   <sheetData>
     <row r="2" spans="7:38" ht="35" customHeight="1">
       <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="J2" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="O2" s="19" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="P2" s="19"/>
       <c r="Q2" s="19"/>
@@ -968,19 +957,19 @@
     </row>
     <row r="3" spans="7:38" ht="35" customHeight="1">
       <c r="H3" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="I3" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>27</v>
-      </c>
       <c r="O3" s="19" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="P3" s="19"/>
       <c r="Q3" s="19"/>
@@ -1004,19 +993,19 @@
     </row>
     <row r="4" spans="7:38" ht="35" customHeight="1">
       <c r="H4" s="10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="O4" s="19" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="P4" s="19"/>
       <c r="Q4" s="19"/>
@@ -1040,19 +1029,19 @@
     </row>
     <row r="5" spans="7:38" ht="35" customHeight="1">
       <c r="H5" s="14" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I5" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="J5" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" s="13" t="s">
-        <v>29</v>
-      </c>
       <c r="O5" s="19" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="P5" s="19"/>
       <c r="Q5" s="19"/>
@@ -1076,25 +1065,31 @@
     </row>
     <row r="7" spans="7:38" ht="35" customHeight="1">
       <c r="H7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="3"/>
+      <c r="J7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="M7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="T7" s="19" t="s">
         <v>0</v>
-      </c>
-      <c r="N7" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="O7" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="P7" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="T7" s="19" t="s">
-        <v>4</v>
       </c>
       <c r="U7" s="19"/>
       <c r="V7" s="19"/>
@@ -1117,17 +1112,31 @@
     <row r="8" spans="7:38" ht="35" customHeight="1">
       <c r="G8" s="18"/>
       <c r="H8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="9"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="9"/>
+        <v>13</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="M8" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="N8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="O8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="P8" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="T8" s="19" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="U8" s="19"/>
       <c r="V8" s="19"/>
@@ -1149,15 +1158,29 @@
     </row>
     <row r="9" spans="7:38" ht="35" customHeight="1">
       <c r="H9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="9"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="9"/>
+        <v>14</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="N9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="O9" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="P9" s="9" t="s">
+        <v>24</v>
+      </c>
       <c r="T9" s="19"/>
       <c r="U9" s="19"/>
       <c r="V9" s="19"/>
@@ -1179,15 +1202,29 @@
     </row>
     <row r="10" spans="7:38" ht="35" customHeight="1">
       <c r="H10" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="13"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="13"/>
+        <v>15</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="K10" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="M10" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="N10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="O10" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="P10" s="13" t="s">
+        <v>25</v>
+      </c>
       <c r="T10" s="19"/>
       <c r="U10" s="19"/>
       <c r="V10" s="19"/>
@@ -1208,16 +1245,32 @@
       <c r="AL10" s="4"/>
     </row>
     <row r="12" spans="7:38" ht="35" customHeight="1">
-      <c r="H12" s="15"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="3"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="3"/>
+      <c r="H12" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="T12" s="19" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="U12" s="19"/>
       <c r="V12" s="19"/>
@@ -1238,14 +1291,30 @@
       <c r="AL12" s="4"/>
     </row>
     <row r="13" spans="7:38" ht="35" customHeight="1">
-      <c r="H13" s="7"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="9"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="16"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="9"/>
+      <c r="H13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N13" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="O13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="P13" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="T13" s="19"/>
       <c r="U13" s="19"/>
       <c r="V13" s="19"/>
@@ -1266,14 +1335,30 @@
       <c r="AL13" s="4"/>
     </row>
     <row r="14" spans="7:38" ht="35" customHeight="1">
-      <c r="H14" s="10"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="9"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="16"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="9"/>
+      <c r="H14" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="M14" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="N14" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="O14" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="P14" s="9" t="s">
+        <v>24</v>
+      </c>
       <c r="T14" s="19"/>
       <c r="U14" s="19"/>
       <c r="V14" s="19"/>
@@ -1294,14 +1379,30 @@
       <c r="AL14" s="4"/>
     </row>
     <row r="15" spans="7:38" ht="35" customHeight="1">
-      <c r="H15" s="14"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="13"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="13"/>
+      <c r="H15" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="K15" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="M15" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="N15" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="O15" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="P15" s="13" t="s">
+        <v>25</v>
+      </c>
       <c r="T15" s="19"/>
       <c r="U15" s="19"/>
       <c r="V15" s="19"/>
@@ -1322,16 +1423,32 @@
       <c r="AL15" s="4"/>
     </row>
     <row r="17" spans="8:38" ht="35" customHeight="1">
-      <c r="H17" s="1"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="3"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="3"/>
+      <c r="H17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M17" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="N17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P17" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="T17" s="19" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="U17" s="19"/>
       <c r="V17" s="19"/>
@@ -1352,14 +1469,30 @@
       <c r="AL17" s="4"/>
     </row>
     <row r="18" spans="8:38" ht="35" customHeight="1">
-      <c r="H18" s="10"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="9"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="16"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="9"/>
+      <c r="H18" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="J18" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="M18" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N18" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="O18" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="P18" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="T18" s="19"/>
       <c r="U18" s="19"/>
       <c r="V18" s="19"/>
@@ -1380,14 +1513,30 @@
       <c r="AL18" s="4"/>
     </row>
     <row r="19" spans="8:38" ht="35" customHeight="1">
-      <c r="H19" s="10"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="9"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="9"/>
+      <c r="H19" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="M19" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="N19" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="O19" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="P19" s="9" t="s">
+        <v>24</v>
+      </c>
       <c r="T19" s="19"/>
       <c r="U19" s="29"/>
       <c r="V19" s="19"/>
@@ -1408,14 +1557,30 @@
       <c r="AL19" s="4"/>
     </row>
     <row r="20" spans="8:38" ht="35" customHeight="1">
-      <c r="H20" s="14"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="13"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="12"/>
-      <c r="O20" s="12"/>
-      <c r="P20" s="13"/>
+      <c r="H20" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J20" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="K20" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="M20" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="N20" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="O20" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="P20" s="13" t="s">
+        <v>25</v>
+      </c>
       <c r="T20" s="19"/>
       <c r="U20" s="19"/>
       <c r="V20" s="19"/>
@@ -1437,333 +1602,621 @@
     </row>
     <row r="22" spans="8:38" ht="35" customHeight="1">
       <c r="H22" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="I22" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I22" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="J22" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="M22" s="15"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
-      <c r="P22" s="3"/>
-      <c r="R22" s="20"/>
-      <c r="S22" s="5"/>
-      <c r="T22" s="5"/>
-      <c r="U22" s="3"/>
-      <c r="W22" s="15"/>
-      <c r="X22" s="2"/>
-      <c r="Y22" s="2"/>
-      <c r="Z22" s="3"/>
+        <v>18</v>
+      </c>
+      <c r="M22" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P22" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="R22" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="S22" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="T22" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="U22" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="W22" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="X22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z22" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="AC22" s="19" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="8:38" ht="35" customHeight="1">
       <c r="H23" s="23" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="I23" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K23" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="J23" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="K23" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="M23" s="7"/>
-      <c r="N23" s="16"/>
-      <c r="O23" s="16"/>
-      <c r="P23" s="9"/>
-      <c r="R23" s="23"/>
-      <c r="S23" s="24"/>
-      <c r="T23" s="16"/>
-      <c r="U23" s="9"/>
-      <c r="W23" s="10"/>
-      <c r="X23" s="8"/>
-      <c r="Y23" s="16"/>
-      <c r="Z23" s="9"/>
+      <c r="M23" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N23" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="O23" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="P23" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="R23" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="S23" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="T23" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="U23" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="W23" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="X23" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y23" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z23" s="9" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="24" spans="8:38" ht="35" customHeight="1">
       <c r="H24" s="23" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I24" s="16" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="J24" s="16" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="K24" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="M24" s="7"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="9"/>
-      <c r="R24" s="23"/>
-      <c r="S24" s="24"/>
-      <c r="T24" s="16"/>
-      <c r="U24" s="9"/>
-      <c r="W24" s="7"/>
-      <c r="X24" s="16"/>
-      <c r="Y24" s="16"/>
-      <c r="Z24" s="9"/>
+        <v>24</v>
+      </c>
+      <c r="M24" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="N24" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="O24" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="P24" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="R24" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="S24" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="T24" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="U24" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="W24" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="X24" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y24" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z24" s="9" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="25" spans="8:38" ht="35" customHeight="1">
       <c r="H25" s="14" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I25" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J25" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="K25" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="J25" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="K25" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="M25" s="14"/>
-      <c r="N25" s="12"/>
-      <c r="O25" s="12"/>
-      <c r="P25" s="13"/>
-      <c r="R25" s="14"/>
-      <c r="S25" s="12"/>
-      <c r="T25" s="12"/>
-      <c r="U25" s="13"/>
-      <c r="W25" s="14"/>
-      <c r="X25" s="12"/>
-      <c r="Y25" s="12"/>
-      <c r="Z25" s="13"/>
+      <c r="M25" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="N25" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="O25" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="P25" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="R25" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="S25" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="T25" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="U25" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="W25" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="X25" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y25" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z25" s="13" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="27" spans="8:38" ht="35" customHeight="1">
       <c r="H27" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="I27" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="I27" s="21" t="s">
-        <v>20</v>
-      </c>
       <c r="J27" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="K27" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="M27" s="20"/>
-      <c r="N27" s="21"/>
-      <c r="O27" s="21"/>
-      <c r="P27" s="22"/>
-      <c r="R27" s="34"/>
-      <c r="S27" s="5"/>
-      <c r="T27" s="5"/>
-      <c r="U27" s="22"/>
-      <c r="W27" s="20"/>
-      <c r="X27" s="21"/>
-      <c r="Y27" s="21"/>
-      <c r="Z27" s="22"/>
+        <v>18</v>
+      </c>
+      <c r="M27" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="N27" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="O27" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="P27" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="R27" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="S27" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="T27" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="U27" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="W27" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="X27" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y27" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z27" s="22" t="s">
+        <v>18</v>
+      </c>
       <c r="AD27" s="19" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="8:38" ht="35" customHeight="1">
       <c r="H28" s="23" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="I28" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="J28" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="K28" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="J28" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="K28" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="M28" s="7"/>
-      <c r="N28" s="24"/>
-      <c r="O28" s="24"/>
-      <c r="P28" s="25"/>
-      <c r="R28" s="23"/>
-      <c r="S28" s="16"/>
-      <c r="T28" s="24"/>
-      <c r="U28" s="25"/>
-      <c r="W28" s="7"/>
-      <c r="X28" s="16"/>
-      <c r="Y28" s="16"/>
-      <c r="Z28" s="25"/>
+      <c r="M28" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N28" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="O28" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="P28" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="R28" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="S28" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="T28" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="U28" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="W28" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="X28" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y28" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z28" s="25" t="s">
+        <v>23</v>
+      </c>
       <c r="AD28" s="19" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="8:38" ht="35" customHeight="1">
       <c r="H29" s="23" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I29" s="16" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="J29" s="16" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="K29" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="M29" s="7"/>
-      <c r="N29" s="16"/>
-      <c r="O29" s="16"/>
-      <c r="P29" s="25"/>
-      <c r="R29" s="23"/>
-      <c r="S29" s="16"/>
-      <c r="T29" s="24"/>
-      <c r="U29" s="25"/>
-      <c r="W29" s="33"/>
-      <c r="X29" s="24"/>
-      <c r="Y29" s="16"/>
-      <c r="Z29" s="25"/>
+        <v>24</v>
+      </c>
+      <c r="M29" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="N29" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="O29" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="P29" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="R29" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="S29" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="T29" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="U29" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="W29" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="X29" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y29" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z29" s="25" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="30" spans="8:38" ht="35" customHeight="1">
       <c r="H30" s="26" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I30" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="J30" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="K30" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="J30" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="K30" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="M30" s="26"/>
-      <c r="N30" s="27"/>
-      <c r="O30" s="27"/>
-      <c r="P30" s="28"/>
-      <c r="R30" s="26"/>
-      <c r="S30" s="27"/>
-      <c r="T30" s="27"/>
-      <c r="U30" s="28"/>
-      <c r="W30" s="26"/>
-      <c r="X30" s="27"/>
-      <c r="Y30" s="27"/>
-      <c r="Z30" s="28"/>
+      <c r="M30" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="N30" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="O30" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="P30" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="R30" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="S30" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="T30" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="U30" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="W30" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="X30" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y30" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z30" s="28" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="32" spans="8:38" ht="35" customHeight="1">
       <c r="H32" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I32" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I32" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="J32" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="M32" s="20"/>
-      <c r="N32" s="5"/>
-      <c r="O32" s="2"/>
-      <c r="P32" s="3"/>
-      <c r="R32" s="1"/>
-      <c r="S32" s="5"/>
-      <c r="T32" s="5"/>
-      <c r="U32" s="3"/>
-      <c r="W32" s="20"/>
-      <c r="X32" s="30"/>
-      <c r="Y32" s="21"/>
-      <c r="Z32" s="22"/>
+        <v>18</v>
+      </c>
+      <c r="M32" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="N32" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="O32" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P32" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="R32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S32" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="T32" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="U32" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="W32" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="X32" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y32" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z32" s="22" t="s">
+        <v>18</v>
+      </c>
       <c r="AC32" s="19" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="8:29" ht="35" customHeight="1">
       <c r="H33" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="I33" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="J33" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="K33" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="J33" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="K33" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="M33" s="23"/>
-      <c r="N33" s="16"/>
-      <c r="O33" s="16"/>
-      <c r="P33" s="9"/>
-      <c r="R33" s="10"/>
-      <c r="S33" s="16"/>
-      <c r="T33" s="8"/>
-      <c r="U33" s="9"/>
-      <c r="W33" s="32"/>
-      <c r="X33" s="31"/>
-      <c r="Y33" s="24"/>
-      <c r="Z33" s="25"/>
+      <c r="M33" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="N33" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="O33" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="P33" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="R33" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="S33" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="T33" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="U33" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="W33" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="X33" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y33" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z33" s="25" t="s">
+        <v>23</v>
+      </c>
       <c r="AC33" s="19" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="8:29" ht="35" customHeight="1">
       <c r="H34" s="10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="J34" s="8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="K34" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="M34" s="23"/>
-      <c r="N34" s="16"/>
-      <c r="O34" s="8"/>
-      <c r="P34" s="9"/>
-      <c r="R34" s="10"/>
-      <c r="S34" s="8"/>
-      <c r="T34" s="8"/>
-      <c r="U34" s="9"/>
-      <c r="W34" s="23"/>
-      <c r="X34" s="31"/>
-      <c r="Y34" s="24"/>
-      <c r="Z34" s="25"/>
+        <v>24</v>
+      </c>
+      <c r="M34" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="N34" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="O34" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="P34" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="R34" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="S34" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="T34" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="U34" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="W34" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="X34" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y34" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z34" s="25" t="s">
+        <v>24</v>
+      </c>
       <c r="AC34" s="19" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="8:29" ht="35" customHeight="1">
       <c r="H35" s="14" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I35" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J35" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="K35" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="J35" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="K35" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="M35" s="14"/>
-      <c r="N35" s="12"/>
-      <c r="O35" s="12"/>
-      <c r="P35" s="13"/>
-      <c r="R35" s="14"/>
-      <c r="S35" s="12"/>
-      <c r="T35" s="12"/>
-      <c r="U35" s="13"/>
-      <c r="W35" s="26"/>
-      <c r="X35" s="27"/>
-      <c r="Y35" s="27"/>
-      <c r="Z35" s="28"/>
+      <c r="M35" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="N35" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="O35" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="P35" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="R35" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="S35" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="T35" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="U35" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="W35" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="X35" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y35" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z35" s="28" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>